<commit_message>
Add feature to upload to MySA
</commit_message>
<xml_diff>
--- a/alfred/tests/resources/alfred/io/question/sample_mcq.xlsx
+++ b/alfred/tests/resources/alfred/io/question/sample_mcq.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11113"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/geoffkoh/Development/github/alfred/alfred/tests/resources/alfred/io/question/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Cindy D Drive\Development\alfred\alfred\tests\resources\alfred\io\question\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{EE6D540A-7C7E-0B44-992E-1502C388D4B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D71BF57B-7C27-4787-A62B-256C7CE0DA2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2660" yWindow="2660" windowWidth="17280" windowHeight="10160" xr2:uid="{5C7A8D2B-F8D8-4943-A545-B08027646AA3}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="17790" xr2:uid="{5C7A8D2B-F8D8-4943-A545-B08027646AA3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="20">
   <si>
     <t>Title</t>
   </si>
@@ -79,14 +79,26 @@
     <t>marks</t>
   </si>
   <si>
-    <t>a</t>
+    <t>A3079C</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>CW1</t>
+  </si>
+  <si>
+    <t>Module Code</t>
+  </si>
+  <si>
+    <t>Assessment Type</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -110,6 +122,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="8"/>
+      <color rgb="FF222222"/>
+      <name val="Verdana"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -131,7 +150,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -187,11 +206,20 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -223,6 +251,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -555,33 +587,34 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF179ADE-5BCD-4579-A68B-F003BDADC528}">
-  <dimension ref="A1:H121"/>
+  <dimension ref="A1:J121"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="15.33203125" customWidth="1"/>
-    <col min="2" max="2" width="43.1640625" style="10" customWidth="1"/>
-    <col min="5" max="5" width="14.5" customWidth="1"/>
+    <col min="2" max="2" width="43.109375" style="10" customWidth="1"/>
+    <col min="5" max="5" width="14.44140625" customWidth="1"/>
+    <col min="10" max="10" width="17.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="A1" s="11" t="s">
+    <row r="1" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="B1" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="15" t="s">
+      <c r="C1" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="15" t="s">
+      <c r="D1" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="E1" s="15" t="s">
+      <c r="E1" s="17" t="s">
         <v>13</v>
       </c>
       <c r="F1" s="6" t="s">
@@ -593,13 +626,19 @@
       <c r="H1" s="6" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="12"/>
-      <c r="B2" s="14"/>
-      <c r="C2" s="16"/>
-      <c r="D2" s="16"/>
-      <c r="E2" s="16"/>
+      <c r="I1" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="J1" s="11" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="14"/>
+      <c r="B2" s="16"/>
+      <c r="C2" s="18"/>
+      <c r="D2" s="18"/>
+      <c r="E2" s="18"/>
       <c r="F2" s="7" t="s">
         <v>14</v>
       </c>
@@ -610,7 +649,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
@@ -631,8 +670,14 @@
       </c>
       <c r="G3" s="2"/>
       <c r="H3" s="2"/>
-    </row>
-    <row r="4" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="I3" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="J3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
         <v>7</v>
       </c>
@@ -646,7 +691,7 @@
       <c r="G4" s="2"/>
       <c r="H4" s="2"/>
     </row>
-    <row r="5" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
         <v>8</v>
       </c>
@@ -657,12 +702,12 @@
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
       <c r="F5" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="G5" s="2"/>
       <c r="H5" s="2"/>
     </row>
-    <row r="6" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
         <v>6</v>
       </c>
@@ -676,7 +721,7 @@
       <c r="G6" s="2"/>
       <c r="H6" s="2"/>
     </row>
-    <row r="7" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="3" t="s">
         <v>5</v>
       </c>
@@ -690,7 +735,7 @@
       <c r="G7" s="2"/>
       <c r="H7" s="2"/>
     </row>
-    <row r="8" spans="1:8" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="4"/>
       <c r="B8" s="9"/>
       <c r="C8" s="5"/>
@@ -700,7 +745,7 @@
       <c r="G8" s="5"/>
       <c r="H8" s="5"/>
     </row>
-    <row r="9" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>9</v>
       </c>
@@ -721,8 +766,14 @@
         <v>1</v>
       </c>
       <c r="H9" s="2"/>
-    </row>
-    <row r="10" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="I9" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="J9" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="3" t="s">
         <v>7</v>
       </c>
@@ -736,7 +787,7 @@
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
     </row>
-    <row r="11" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="3" t="s">
         <v>8</v>
       </c>
@@ -750,7 +801,7 @@
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
     </row>
-    <row r="12" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="3" t="s">
         <v>6</v>
       </c>
@@ -764,7 +815,7 @@
       <c r="G12" s="2"/>
       <c r="H12" s="2"/>
     </row>
-    <row r="13" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="3" t="s">
         <v>5</v>
       </c>
@@ -778,7 +829,7 @@
       <c r="G13" s="2"/>
       <c r="H13" s="2"/>
     </row>
-    <row r="14" spans="1:8" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="4"/>
       <c r="B14" s="9"/>
       <c r="C14" s="5"/>
@@ -788,7 +839,7 @@
       <c r="G14" s="5"/>
       <c r="H14" s="5"/>
     </row>
-    <row r="15" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
         <v>11</v>
       </c>
@@ -809,8 +860,14 @@
       <c r="H15" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="16" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="I15" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="J15" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="3" t="s">
         <v>7</v>
       </c>
@@ -824,7 +881,7 @@
       <c r="G16" s="2"/>
       <c r="H16" s="2"/>
     </row>
-    <row r="17" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="3" t="s">
         <v>8</v>
       </c>
@@ -838,7 +895,7 @@
       <c r="G17" s="2"/>
       <c r="H17" s="2"/>
     </row>
-    <row r="18" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="3" t="s">
         <v>6</v>
       </c>
@@ -852,7 +909,7 @@
       <c r="G18" s="2"/>
       <c r="H18" s="2"/>
     </row>
-    <row r="19" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="3" t="s">
         <v>5</v>
       </c>
@@ -866,7 +923,7 @@
       <c r="G19" s="2"/>
       <c r="H19" s="2"/>
     </row>
-    <row r="20" spans="1:8" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="4"/>
       <c r="B20" s="9"/>
       <c r="C20" s="5"/>
@@ -876,7 +933,7 @@
       <c r="G20" s="5"/>
       <c r="H20" s="5"/>
     </row>
-    <row r="21" spans="1:8" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="1"/>
       <c r="B21" s="8"/>
       <c r="C21" s="2"/>
@@ -886,7 +943,7 @@
       <c r="G21" s="2"/>
       <c r="H21" s="2"/>
     </row>
-    <row r="22" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A22" s="3" t="s">
         <v>7</v>
       </c>
@@ -898,7 +955,7 @@
       <c r="G22" s="2"/>
       <c r="H22" s="2"/>
     </row>
-    <row r="23" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" s="3" t="s">
         <v>8</v>
       </c>
@@ -910,7 +967,7 @@
       <c r="G23" s="2"/>
       <c r="H23" s="2"/>
     </row>
-    <row r="24" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A24" s="3" t="s">
         <v>6</v>
       </c>
@@ -922,7 +979,7 @@
       <c r="G24" s="2"/>
       <c r="H24" s="2"/>
     </row>
-    <row r="25" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A25" s="3" t="s">
         <v>5</v>
       </c>
@@ -934,7 +991,7 @@
       <c r="G25" s="2"/>
       <c r="H25" s="2"/>
     </row>
-    <row r="26" spans="1:8" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A26" s="4"/>
       <c r="B26" s="9"/>
       <c r="C26" s="5"/>
@@ -944,7 +1001,7 @@
       <c r="G26" s="5"/>
       <c r="H26" s="5"/>
     </row>
-    <row r="27" spans="1:8" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A27" s="1"/>
       <c r="B27" s="8"/>
       <c r="C27" s="2"/>
@@ -954,7 +1011,7 @@
       <c r="G27" s="2"/>
       <c r="H27" s="2"/>
     </row>
-    <row r="28" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A28" s="3" t="s">
         <v>7</v>
       </c>
@@ -966,7 +1023,7 @@
       <c r="G28" s="2"/>
       <c r="H28" s="2"/>
     </row>
-    <row r="29" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A29" s="3" t="s">
         <v>8</v>
       </c>
@@ -978,7 +1035,7 @@
       <c r="G29" s="2"/>
       <c r="H29" s="2"/>
     </row>
-    <row r="30" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A30" s="3" t="s">
         <v>6</v>
       </c>
@@ -990,7 +1047,7 @@
       <c r="G30" s="2"/>
       <c r="H30" s="2"/>
     </row>
-    <row r="31" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A31" s="3" t="s">
         <v>5</v>
       </c>
@@ -1002,7 +1059,7 @@
       <c r="G31" s="2"/>
       <c r="H31" s="2"/>
     </row>
-    <row r="32" spans="1:8" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A32" s="4"/>
       <c r="B32" s="9"/>
       <c r="C32" s="5"/>
@@ -1012,7 +1069,7 @@
       <c r="G32" s="5"/>
       <c r="H32" s="5"/>
     </row>
-    <row r="33" spans="1:8" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A33" s="1"/>
       <c r="B33" s="8"/>
       <c r="C33" s="2"/>
@@ -1022,7 +1079,7 @@
       <c r="G33" s="2"/>
       <c r="H33" s="2"/>
     </row>
-    <row r="34" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A34" s="3" t="s">
         <v>7</v>
       </c>
@@ -1034,7 +1091,7 @@
       <c r="G34" s="2"/>
       <c r="H34" s="2"/>
     </row>
-    <row r="35" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A35" s="3" t="s">
         <v>8</v>
       </c>
@@ -1046,7 +1103,7 @@
       <c r="G35" s="2"/>
       <c r="H35" s="2"/>
     </row>
-    <row r="36" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A36" s="3" t="s">
         <v>6</v>
       </c>
@@ -1058,7 +1115,7 @@
       <c r="G36" s="2"/>
       <c r="H36" s="2"/>
     </row>
-    <row r="37" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A37" s="3" t="s">
         <v>5</v>
       </c>
@@ -1070,7 +1127,7 @@
       <c r="G37" s="2"/>
       <c r="H37" s="2"/>
     </row>
-    <row r="38" spans="1:8" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A38" s="4"/>
       <c r="B38" s="9"/>
       <c r="C38" s="5"/>
@@ -1080,7 +1137,7 @@
       <c r="G38" s="5"/>
       <c r="H38" s="5"/>
     </row>
-    <row r="39" spans="1:8" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A39" s="1"/>
       <c r="B39" s="8"/>
       <c r="C39" s="2"/>
@@ -1090,7 +1147,7 @@
       <c r="G39" s="2"/>
       <c r="H39" s="2"/>
     </row>
-    <row r="40" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A40" s="3" t="s">
         <v>7</v>
       </c>
@@ -1102,7 +1159,7 @@
       <c r="G40" s="2"/>
       <c r="H40" s="2"/>
     </row>
-    <row r="41" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A41" s="3" t="s">
         <v>8</v>
       </c>
@@ -1114,7 +1171,7 @@
       <c r="G41" s="2"/>
       <c r="H41" s="2"/>
     </row>
-    <row r="42" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A42" s="3" t="s">
         <v>6</v>
       </c>
@@ -1126,7 +1183,7 @@
       <c r="G42" s="2"/>
       <c r="H42" s="2"/>
     </row>
-    <row r="43" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A43" s="3" t="s">
         <v>5</v>
       </c>
@@ -1138,7 +1195,7 @@
       <c r="G43" s="2"/>
       <c r="H43" s="2"/>
     </row>
-    <row r="44" spans="1:8" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A44" s="4"/>
       <c r="B44" s="9"/>
       <c r="C44" s="5"/>
@@ -1148,7 +1205,7 @@
       <c r="G44" s="5"/>
       <c r="H44" s="5"/>
     </row>
-    <row r="45" spans="1:8" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A45" s="1"/>
       <c r="B45" s="8"/>
       <c r="C45" s="2"/>
@@ -1158,7 +1215,7 @@
       <c r="G45" s="2"/>
       <c r="H45" s="2"/>
     </row>
-    <row r="46" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A46" s="3" t="s">
         <v>7</v>
       </c>
@@ -1170,7 +1227,7 @@
       <c r="G46" s="2"/>
       <c r="H46" s="2"/>
     </row>
-    <row r="47" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A47" s="3" t="s">
         <v>8</v>
       </c>
@@ -1182,7 +1239,7 @@
       <c r="G47" s="2"/>
       <c r="H47" s="2"/>
     </row>
-    <row r="48" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A48" s="3" t="s">
         <v>6</v>
       </c>
@@ -1194,7 +1251,7 @@
       <c r="G48" s="2"/>
       <c r="H48" s="2"/>
     </row>
-    <row r="49" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A49" s="3" t="s">
         <v>5</v>
       </c>
@@ -1206,7 +1263,7 @@
       <c r="G49" s="2"/>
       <c r="H49" s="2"/>
     </row>
-    <row r="50" spans="1:8" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A50" s="4"/>
       <c r="B50" s="9"/>
       <c r="C50" s="5"/>
@@ -1216,7 +1273,7 @@
       <c r="G50" s="5"/>
       <c r="H50" s="5"/>
     </row>
-    <row r="51" spans="1:8" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A51" s="1"/>
       <c r="B51" s="8"/>
       <c r="C51" s="2"/>
@@ -1226,7 +1283,7 @@
       <c r="G51" s="2"/>
       <c r="H51" s="2"/>
     </row>
-    <row r="52" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A52" s="3" t="s">
         <v>7</v>
       </c>
@@ -1238,7 +1295,7 @@
       <c r="G52" s="2"/>
       <c r="H52" s="2"/>
     </row>
-    <row r="53" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A53" s="3" t="s">
         <v>8</v>
       </c>
@@ -1250,7 +1307,7 @@
       <c r="G53" s="2"/>
       <c r="H53" s="2"/>
     </row>
-    <row r="54" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A54" s="3" t="s">
         <v>6</v>
       </c>
@@ -1262,7 +1319,7 @@
       <c r="G54" s="2"/>
       <c r="H54" s="2"/>
     </row>
-    <row r="55" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A55" s="3" t="s">
         <v>5</v>
       </c>
@@ -1274,7 +1331,7 @@
       <c r="G55" s="2"/>
       <c r="H55" s="2"/>
     </row>
-    <row r="56" spans="1:8" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A56" s="4"/>
       <c r="B56" s="9"/>
       <c r="C56" s="5"/>
@@ -1284,7 +1341,7 @@
       <c r="G56" s="5"/>
       <c r="H56" s="5"/>
     </row>
-    <row r="57" spans="1:8" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A57" s="1"/>
       <c r="B57" s="8"/>
       <c r="C57" s="2"/>
@@ -1294,7 +1351,7 @@
       <c r="G57" s="2"/>
       <c r="H57" s="2"/>
     </row>
-    <row r="58" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A58" s="3" t="s">
         <v>7</v>
       </c>
@@ -1306,7 +1363,7 @@
       <c r="G58" s="2"/>
       <c r="H58" s="2"/>
     </row>
-    <row r="59" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A59" s="3" t="s">
         <v>8</v>
       </c>
@@ -1318,7 +1375,7 @@
       <c r="G59" s="2"/>
       <c r="H59" s="2"/>
     </row>
-    <row r="60" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A60" s="3" t="s">
         <v>6</v>
       </c>
@@ -1330,7 +1387,7 @@
       <c r="G60" s="2"/>
       <c r="H60" s="2"/>
     </row>
-    <row r="61" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A61" s="3" t="s">
         <v>5</v>
       </c>
@@ -1342,7 +1399,7 @@
       <c r="G61" s="2"/>
       <c r="H61" s="2"/>
     </row>
-    <row r="62" spans="1:8" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A62" s="4"/>
       <c r="B62" s="9"/>
       <c r="C62" s="5"/>
@@ -1352,7 +1409,7 @@
       <c r="G62" s="5"/>
       <c r="H62" s="5"/>
     </row>
-    <row r="63" spans="1:8" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A63" s="1"/>
       <c r="B63" s="8"/>
       <c r="C63" s="2"/>
@@ -1362,7 +1419,7 @@
       <c r="G63" s="2"/>
       <c r="H63" s="2"/>
     </row>
-    <row r="64" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A64" s="3" t="s">
         <v>7</v>
       </c>
@@ -1374,7 +1431,7 @@
       <c r="G64" s="2"/>
       <c r="H64" s="2"/>
     </row>
-    <row r="65" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A65" s="3" t="s">
         <v>8</v>
       </c>
@@ -1386,7 +1443,7 @@
       <c r="G65" s="2"/>
       <c r="H65" s="2"/>
     </row>
-    <row r="66" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A66" s="3" t="s">
         <v>6</v>
       </c>
@@ -1398,7 +1455,7 @@
       <c r="G66" s="2"/>
       <c r="H66" s="2"/>
     </row>
-    <row r="67" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A67" s="3" t="s">
         <v>5</v>
       </c>
@@ -1410,7 +1467,7 @@
       <c r="G67" s="2"/>
       <c r="H67" s="2"/>
     </row>
-    <row r="68" spans="1:8" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A68" s="4"/>
       <c r="B68" s="9"/>
       <c r="C68" s="5"/>
@@ -1420,7 +1477,7 @@
       <c r="G68" s="5"/>
       <c r="H68" s="5"/>
     </row>
-    <row r="69" spans="1:8" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A69" s="1"/>
       <c r="B69" s="8"/>
       <c r="C69" s="2"/>
@@ -1430,7 +1487,7 @@
       <c r="G69" s="2"/>
       <c r="H69" s="2"/>
     </row>
-    <row r="70" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A70" s="3" t="s">
         <v>7</v>
       </c>
@@ -1442,7 +1499,7 @@
       <c r="G70" s="2"/>
       <c r="H70" s="2"/>
     </row>
-    <row r="71" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A71" s="3" t="s">
         <v>8</v>
       </c>
@@ -1454,7 +1511,7 @@
       <c r="G71" s="2"/>
       <c r="H71" s="2"/>
     </row>
-    <row r="72" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A72" s="3" t="s">
         <v>6</v>
       </c>
@@ -1466,7 +1523,7 @@
       <c r="G72" s="2"/>
       <c r="H72" s="2"/>
     </row>
-    <row r="73" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A73" s="3" t="s">
         <v>5</v>
       </c>
@@ -1478,7 +1535,7 @@
       <c r="G73" s="2"/>
       <c r="H73" s="2"/>
     </row>
-    <row r="74" spans="1:8" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A74" s="4"/>
       <c r="B74" s="9"/>
       <c r="C74" s="5"/>
@@ -1488,7 +1545,7 @@
       <c r="G74" s="5"/>
       <c r="H74" s="5"/>
     </row>
-    <row r="75" spans="1:8" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A75" s="1"/>
       <c r="B75" s="8"/>
       <c r="C75" s="2"/>
@@ -1498,7 +1555,7 @@
       <c r="G75" s="2"/>
       <c r="H75" s="2"/>
     </row>
-    <row r="76" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A76" s="3" t="s">
         <v>7</v>
       </c>
@@ -1510,7 +1567,7 @@
       <c r="G76" s="2"/>
       <c r="H76" s="2"/>
     </row>
-    <row r="77" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A77" s="3" t="s">
         <v>8</v>
       </c>
@@ -1522,7 +1579,7 @@
       <c r="G77" s="2"/>
       <c r="H77" s="2"/>
     </row>
-    <row r="78" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A78" s="3" t="s">
         <v>6</v>
       </c>
@@ -1534,7 +1591,7 @@
       <c r="G78" s="2"/>
       <c r="H78" s="2"/>
     </row>
-    <row r="79" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A79" s="3" t="s">
         <v>5</v>
       </c>
@@ -1546,7 +1603,7 @@
       <c r="G79" s="2"/>
       <c r="H79" s="2"/>
     </row>
-    <row r="80" spans="1:8" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A80" s="4"/>
       <c r="B80" s="9"/>
       <c r="C80" s="5"/>
@@ -1556,7 +1613,7 @@
       <c r="G80" s="5"/>
       <c r="H80" s="5"/>
     </row>
-    <row r="81" spans="1:8" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A81" s="1"/>
       <c r="B81" s="8"/>
       <c r="C81" s="2"/>
@@ -1566,7 +1623,7 @@
       <c r="G81" s="2"/>
       <c r="H81" s="2"/>
     </row>
-    <row r="82" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A82" s="3" t="s">
         <v>7</v>
       </c>
@@ -1578,7 +1635,7 @@
       <c r="G82" s="2"/>
       <c r="H82" s="2"/>
     </row>
-    <row r="83" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A83" s="3" t="s">
         <v>8</v>
       </c>
@@ -1590,7 +1647,7 @@
       <c r="G83" s="2"/>
       <c r="H83" s="2"/>
     </row>
-    <row r="84" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A84" s="3" t="s">
         <v>6</v>
       </c>
@@ -1602,7 +1659,7 @@
       <c r="G84" s="2"/>
       <c r="H84" s="2"/>
     </row>
-    <row r="85" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A85" s="3" t="s">
         <v>5</v>
       </c>
@@ -1614,7 +1671,7 @@
       <c r="G85" s="2"/>
       <c r="H85" s="2"/>
     </row>
-    <row r="86" spans="1:8" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A86" s="4"/>
       <c r="B86" s="9"/>
       <c r="C86" s="5"/>
@@ -1624,7 +1681,7 @@
       <c r="G86" s="5"/>
       <c r="H86" s="5"/>
     </row>
-    <row r="87" spans="1:8" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A87" s="1"/>
       <c r="B87" s="8"/>
       <c r="C87" s="2"/>
@@ -1634,7 +1691,7 @@
       <c r="G87" s="2"/>
       <c r="H87" s="2"/>
     </row>
-    <row r="88" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A88" s="3" t="s">
         <v>7</v>
       </c>
@@ -1646,7 +1703,7 @@
       <c r="G88" s="2"/>
       <c r="H88" s="2"/>
     </row>
-    <row r="89" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A89" s="3" t="s">
         <v>8</v>
       </c>
@@ -1658,7 +1715,7 @@
       <c r="G89" s="2"/>
       <c r="H89" s="2"/>
     </row>
-    <row r="90" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A90" s="3" t="s">
         <v>6</v>
       </c>
@@ -1670,7 +1727,7 @@
       <c r="G90" s="2"/>
       <c r="H90" s="2"/>
     </row>
-    <row r="91" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A91" s="3" t="s">
         <v>5</v>
       </c>
@@ -1682,7 +1739,7 @@
       <c r="G91" s="2"/>
       <c r="H91" s="2"/>
     </row>
-    <row r="92" spans="1:8" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A92" s="4"/>
       <c r="B92" s="9"/>
       <c r="C92" s="5"/>
@@ -1692,7 +1749,7 @@
       <c r="G92" s="5"/>
       <c r="H92" s="5"/>
     </row>
-    <row r="93" spans="1:8" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A93" s="1"/>
       <c r="B93" s="8"/>
       <c r="C93" s="2"/>
@@ -1702,7 +1759,7 @@
       <c r="G93" s="2"/>
       <c r="H93" s="2"/>
     </row>
-    <row r="94" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A94" s="3" t="s">
         <v>7</v>
       </c>
@@ -1714,7 +1771,7 @@
       <c r="G94" s="2"/>
       <c r="H94" s="2"/>
     </row>
-    <row r="95" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A95" s="3" t="s">
         <v>8</v>
       </c>
@@ -1726,7 +1783,7 @@
       <c r="G95" s="2"/>
       <c r="H95" s="2"/>
     </row>
-    <row r="96" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A96" s="3" t="s">
         <v>6</v>
       </c>
@@ -1738,7 +1795,7 @@
       <c r="G96" s="2"/>
       <c r="H96" s="2"/>
     </row>
-    <row r="97" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A97" s="3" t="s">
         <v>5</v>
       </c>
@@ -1750,7 +1807,7 @@
       <c r="G97" s="2"/>
       <c r="H97" s="2"/>
     </row>
-    <row r="98" spans="1:8" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A98" s="4"/>
       <c r="B98" s="9"/>
       <c r="C98" s="5"/>
@@ -1760,7 +1817,7 @@
       <c r="G98" s="5"/>
       <c r="H98" s="5"/>
     </row>
-    <row r="99" spans="1:8" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A99" s="1"/>
       <c r="B99" s="8"/>
       <c r="C99" s="2"/>
@@ -1770,7 +1827,7 @@
       <c r="G99" s="2"/>
       <c r="H99" s="2"/>
     </row>
-    <row r="100" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A100" s="3" t="s">
         <v>7</v>
       </c>
@@ -1782,7 +1839,7 @@
       <c r="G100" s="2"/>
       <c r="H100" s="2"/>
     </row>
-    <row r="101" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A101" s="3" t="s">
         <v>8</v>
       </c>
@@ -1794,7 +1851,7 @@
       <c r="G101" s="2"/>
       <c r="H101" s="2"/>
     </row>
-    <row r="102" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A102" s="3" t="s">
         <v>6</v>
       </c>
@@ -1806,7 +1863,7 @@
       <c r="G102" s="2"/>
       <c r="H102" s="2"/>
     </row>
-    <row r="103" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A103" s="3" t="s">
         <v>5</v>
       </c>
@@ -1818,7 +1875,7 @@
       <c r="G103" s="2"/>
       <c r="H103" s="2"/>
     </row>
-    <row r="104" spans="1:8" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A104" s="4"/>
       <c r="B104" s="9"/>
       <c r="C104" s="5"/>
@@ -1828,7 +1885,7 @@
       <c r="G104" s="5"/>
       <c r="H104" s="5"/>
     </row>
-    <row r="105" spans="1:8" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A105" s="1"/>
       <c r="B105" s="8"/>
       <c r="C105" s="2"/>
@@ -1838,7 +1895,7 @@
       <c r="G105" s="2"/>
       <c r="H105" s="2"/>
     </row>
-    <row r="106" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A106" s="3" t="s">
         <v>7</v>
       </c>
@@ -1850,7 +1907,7 @@
       <c r="G106" s="2"/>
       <c r="H106" s="2"/>
     </row>
-    <row r="107" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A107" s="3" t="s">
         <v>8</v>
       </c>
@@ -1862,7 +1919,7 @@
       <c r="G107" s="2"/>
       <c r="H107" s="2"/>
     </row>
-    <row r="108" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A108" s="3" t="s">
         <v>6</v>
       </c>
@@ -1874,7 +1931,7 @@
       <c r="G108" s="2"/>
       <c r="H108" s="2"/>
     </row>
-    <row r="109" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A109" s="3" t="s">
         <v>5</v>
       </c>
@@ -1886,7 +1943,7 @@
       <c r="G109" s="2"/>
       <c r="H109" s="2"/>
     </row>
-    <row r="110" spans="1:8" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A110" s="4"/>
       <c r="B110" s="9"/>
       <c r="C110" s="5"/>
@@ -1896,7 +1953,7 @@
       <c r="G110" s="5"/>
       <c r="H110" s="5"/>
     </row>
-    <row r="111" spans="1:8" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A111" s="1"/>
       <c r="B111" s="8"/>
       <c r="C111" s="2"/>
@@ -1906,7 +1963,7 @@
       <c r="G111" s="2"/>
       <c r="H111" s="2"/>
     </row>
-    <row r="112" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A112" s="3" t="s">
         <v>7</v>
       </c>
@@ -1918,7 +1975,7 @@
       <c r="G112" s="2"/>
       <c r="H112" s="2"/>
     </row>
-    <row r="113" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A113" s="3" t="s">
         <v>8</v>
       </c>
@@ -1930,7 +1987,7 @@
       <c r="G113" s="2"/>
       <c r="H113" s="2"/>
     </row>
-    <row r="114" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A114" s="3" t="s">
         <v>6</v>
       </c>
@@ -1942,7 +1999,7 @@
       <c r="G114" s="2"/>
       <c r="H114" s="2"/>
     </row>
-    <row r="115" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A115" s="3" t="s">
         <v>5</v>
       </c>
@@ -1954,7 +2011,7 @@
       <c r="G115" s="2"/>
       <c r="H115" s="2"/>
     </row>
-    <row r="116" spans="1:8" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A116" s="4"/>
       <c r="B116" s="9"/>
       <c r="C116" s="5"/>
@@ -1964,7 +2021,7 @@
       <c r="G116" s="5"/>
       <c r="H116" s="5"/>
     </row>
-    <row r="117" spans="1:8" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A117" s="1"/>
       <c r="B117" s="8"/>
       <c r="C117" s="2"/>
@@ -1974,7 +2031,7 @@
       <c r="G117" s="2"/>
       <c r="H117" s="2"/>
     </row>
-    <row r="118" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A118" s="3" t="s">
         <v>7</v>
       </c>
@@ -1986,7 +2043,7 @@
       <c r="G118" s="2"/>
       <c r="H118" s="2"/>
     </row>
-    <row r="119" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A119" s="3" t="s">
         <v>8</v>
       </c>
@@ -1998,7 +2055,7 @@
       <c r="G119" s="2"/>
       <c r="H119" s="2"/>
     </row>
-    <row r="120" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A120" s="3" t="s">
         <v>6</v>
       </c>
@@ -2010,7 +2067,7 @@
       <c r="G120" s="2"/>
       <c r="H120" s="2"/>
     </row>
-    <row r="121" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A121" s="3" t="s">
         <v>5</v>
       </c>

</xml_diff>